<commit_message>
grid edit n email
</commit_message>
<xml_diff>
--- a/branches/FaizanTasks.xlsx
+++ b/branches/FaizanTasks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="15600" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
   <si>
     <t>Tasks</t>
   </si>
@@ -100,9 +100,6 @@
   </si>
   <si>
     <t>Issues With PO and DN Help</t>
-  </si>
-  <si>
-    <t>Problem</t>
   </si>
   <si>
     <t>Completed</t>
@@ -466,8 +463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -534,7 +531,7 @@
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>25</v>
@@ -542,7 +539,9 @@
       <c r="H2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="2"/>
+      <c r="I2" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
@@ -556,10 +555,18 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
+      <c r="F3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
@@ -573,10 +580,18 @@
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
@@ -597,7 +612,7 @@
         <v>41941</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>25</v>
@@ -621,7 +636,9 @@
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="F6" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>

</xml_diff>